<commit_message>
GDE-9328: pushed latest dataset
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_ATM_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_ATM_BILAT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE49B110-0E1A-4F7A-A8B9-184B5B7FC25F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68026BCD-00A9-4433-9579-3D28C217172B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="737" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5361,7 +5361,7 @@
   <dimension ref="A1:AS7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AN1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="AS5" sqref="AS5"/>
+      <selection activeCell="AS1" sqref="AS1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
GDE-9328: updated dataset, addressed review points
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_ATM_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_ATM_BILAT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68026BCD-00A9-4433-9579-3D28C217172B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DA5E85-03B9-48A1-B369-A5AB9488F2C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="737" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="638">
   <si>
     <t>rowid</t>
   </si>
@@ -1954,12 +1954,6 @@
   </si>
   <si>
     <t>Primary_PercentOfDeal</t>
-  </si>
-  <si>
-    <t>LineFee_Release_Status</t>
-  </si>
-  <si>
-    <t>Released</t>
   </si>
 </sst>
 </file>
@@ -5358,10 +5352,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:AS7"/>
+  <dimension ref="A1:AR7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AN1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="AS1" sqref="AS1"/>
+      <selection activeCell="AS1" sqref="AS1:AS1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5403,10 +5397,9 @@
     <col min="41" max="41" width="21" style="59" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="22" style="59" bestFit="1" customWidth="1"/>
     <col min="43" max="44" width="26.7109375" style="59" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="39" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:44" s="39" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
@@ -5539,11 +5532,8 @@
       <c r="AR1" s="39" t="s">
         <v>511</v>
       </c>
-      <c r="AS1" s="39" t="s">
-        <v>638</v>
-      </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -5672,11 +5662,8 @@
       <c r="AR2" s="44" t="s">
         <v>533</v>
       </c>
-      <c r="AS2" t="s">
-        <v>639</v>
-      </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="R7" s="37"/>
       <c r="S7" s="37"/>
       <c r="T7" s="37"/>

</xml_diff>

<commit_message>
GDE-9517: corrected replace variables
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_ATM_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_ATM_BILAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6550EAAF-4582-47F6-A613-7D049141FCAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1888A2A4-65F4-416E-AEBA-1B6B4DCDB89C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="737" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="737" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="674">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="666">
   <si>
     <t>rowid</t>
   </si>
@@ -2014,31 +2014,7 @@
     <t>Cycles_ForLoan</t>
   </si>
   <si>
-    <t>Interest_OptionType</t>
-  </si>
-  <si>
-    <t>Loan_InterestAmount</t>
-  </si>
-  <si>
-    <t>Principal_OptionType</t>
-  </si>
-  <si>
-    <t>Breakfunding_Reason</t>
-  </si>
-  <si>
     <t>Paper Clip Payment</t>
-  </si>
-  <si>
-    <t>BBSW/Interest</t>
-  </si>
-  <si>
-    <t>412.25</t>
-  </si>
-  <si>
-    <t>BBSW/Principal</t>
-  </si>
-  <si>
-    <t>Borrower Decision</t>
   </si>
   <si>
     <t>SERV23_LoanPaperClip_ATM_BILAT_OUTSTANDING_B</t>
@@ -3692,10 +3668,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3708,14 +3684,13 @@
     <col min="7" max="7" width="25" style="97" customWidth="1"/>
     <col min="8" max="8" width="28" style="97" customWidth="1"/>
     <col min="9" max="9" width="37" style="97" bestFit="1" customWidth="1"/>
-    <col min="10" max="16" width="26.28515625" style="97" customWidth="1"/>
-    <col min="17" max="17" width="22" style="97" customWidth="1"/>
-    <col min="18" max="18" width="30.28515625" style="97" customWidth="1"/>
-    <col min="19" max="19" width="23.140625" style="97" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="97"/>
+    <col min="10" max="13" width="26.28515625" style="97" customWidth="1"/>
+    <col min="14" max="14" width="22" style="97" customWidth="1"/>
+    <col min="15" max="15" width="30.28515625" style="97" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="97"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="94" t="s">
         <v>0</v>
       </c>
@@ -3732,7 +3707,7 @@
         <v>654</v>
       </c>
       <c r="F1" s="94" t="s">
-        <v>669</v>
+        <v>661</v>
       </c>
       <c r="G1" s="94" t="s">
         <v>655</v>
@@ -3741,7 +3716,7 @@
         <v>611</v>
       </c>
       <c r="I1" s="94" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
       <c r="J1" s="95" t="s">
         <v>656</v>
@@ -3750,57 +3725,45 @@
         <v>535</v>
       </c>
       <c r="L1" s="95" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
       <c r="M1" s="95" t="s">
         <v>609</v>
       </c>
-      <c r="N1" s="95" t="s">
-        <v>657</v>
-      </c>
-      <c r="O1" s="95" t="s">
-        <v>658</v>
-      </c>
-      <c r="P1" s="95" t="s">
-        <v>659</v>
-      </c>
-      <c r="Q1" s="96" t="s">
+      <c r="N1" s="96" t="s">
         <v>552</v>
       </c>
-      <c r="R1" s="96" t="s">
+      <c r="O1" s="96" t="s">
         <v>196</v>
       </c>
-      <c r="S1" s="96" t="s">
-        <v>660</v>
-      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="98" t="s">
         <v>94</v>
       </c>
       <c r="B2" s="98" t="s">
-        <v>666</v>
+        <v>658</v>
       </c>
       <c r="C2" s="98" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="D2" s="98" t="s">
-        <v>667</v>
+        <v>659</v>
       </c>
       <c r="E2" s="99" t="s">
         <v>652</v>
       </c>
       <c r="F2" s="99" t="s">
-        <v>668</v>
+        <v>660</v>
       </c>
       <c r="G2" s="99" t="s">
-        <v>668</v>
+        <v>660</v>
       </c>
       <c r="H2" s="100" t="s">
         <v>651</v>
       </c>
       <c r="I2" s="100" t="s">
-        <v>672</v>
+        <v>664</v>
       </c>
       <c r="J2" s="100" t="s">
         <v>577</v>
@@ -3809,45 +3772,27 @@
         <v>539</v>
       </c>
       <c r="L2" s="104" t="s">
-        <v>671</v>
+        <v>663</v>
       </c>
       <c r="M2" s="99" t="s">
         <v>472</v>
       </c>
-      <c r="N2" s="99" t="s">
-        <v>662</v>
-      </c>
-      <c r="O2" s="99" t="s">
-        <v>663</v>
-      </c>
-      <c r="P2" s="99" t="s">
-        <v>664</v>
-      </c>
-      <c r="Q2" s="98" t="s">
+      <c r="N2" s="98" t="s">
         <v>139</v>
       </c>
-      <c r="R2" s="98" t="s">
+      <c r="O2" s="98" t="s">
         <v>139</v>
       </c>
-      <c r="S2" s="98" t="s">
-        <v>665</v>
-      </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="L9" s="101"/>
       <c r="M9" s="101"/>
-      <c r="N9" s="101"/>
-      <c r="O9" s="101"/>
-      <c r="P9" s="101"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="J10" s="102"/>
       <c r="K10" s="102"/>
       <c r="L10" s="102"/>
       <c r="M10" s="102"/>
-      <c r="N10" s="102"/>
-      <c r="O10" s="102"/>
-      <c r="P10" s="102"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5712,8 +5657,8 @@
   </sheetPr>
   <dimension ref="A1:AY7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="AC1" sqref="AC1"/>
+    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5952,19 +5897,19 @@
       <c r="L2" s="65" t="s">
         <v>514</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="M2" s="46" t="s">
         <v>515</v>
       </c>
-      <c r="N2" s="35" t="s">
+      <c r="N2" s="46" t="s">
         <v>516</v>
       </c>
-      <c r="O2" s="35" t="s">
+      <c r="O2" s="46" t="s">
         <v>515</v>
       </c>
       <c r="P2" s="65" t="s">
         <v>517</v>
       </c>
-      <c r="Q2" s="35" t="s">
+      <c r="Q2" s="46" t="s">
         <v>518</v>
       </c>
       <c r="R2" s="46" t="s">
@@ -6070,13 +6015,13 @@
       <c r="AT3" s="103" t="s">
         <v>94</v>
       </c>
-      <c r="AU3" s="35" t="s">
+      <c r="AU3" s="46" t="s">
         <v>515</v>
       </c>
-      <c r="AV3" s="35" t="s">
+      <c r="AV3" s="46" t="s">
         <v>518</v>
       </c>
-      <c r="AW3" s="35" t="s">
+      <c r="AW3" s="46" t="s">
         <v>515</v>
       </c>
       <c r="AX3" s="93" t="s">
@@ -6668,7 +6613,7 @@
   </sheetPr>
   <dimension ref="A1:AL3"/>
   <sheetViews>
-    <sheetView topLeftCell="AA1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
       <selection activeCell="AK1" sqref="AK1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
GDE-9517: downloaded updated dataset and applied my changes
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_ATM_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_ATM_BILAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1888A2A4-65F4-416E-AEBA-1B6B4DCDB89C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4933291-FFFC-4C85-A507-A692A33EDA06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="737" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="737" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="666">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="674">
   <si>
     <t>rowid</t>
   </si>
@@ -2039,6 +2039,30 @@
   </si>
   <si>
     <t>Paperclip_Total_Prepayment_Amount</t>
+  </si>
+  <si>
+    <t>60003082</t>
+  </si>
+  <si>
+    <t>21-Sep-2019</t>
+  </si>
+  <si>
+    <t>30-Jun-2025</t>
+  </si>
+  <si>
+    <t>3 Months</t>
+  </si>
+  <si>
+    <t>30-Dec-2019</t>
+  </si>
+  <si>
+    <t>0.970000%</t>
+  </si>
+  <si>
+    <t>2.370000%</t>
+  </si>
+  <si>
+    <t>Quarterly</t>
   </si>
 </sst>
 </file>
@@ -2264,7 +2288,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2442,6 +2466,9 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="4" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5657,8 +5684,8 @@
   </sheetPr>
   <dimension ref="A1:AY7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6613,8 +6640,8 @@
   </sheetPr>
   <dimension ref="A1:AL3"/>
   <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="AK1" sqref="AK1"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6787,21 +6814,79 @@
       <c r="E2" s="65" t="s">
         <v>351</v>
       </c>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="Q2" s="86"/>
-      <c r="U2" s="86"/>
-      <c r="V2" s="86"/>
-      <c r="W2" s="86"/>
-      <c r="X2" s="86"/>
-      <c r="Y2" s="86"/>
-      <c r="Z2" s="86"/>
-      <c r="AA2" s="86"/>
-      <c r="AE2" s="87"/>
-      <c r="AF2" s="49"/>
+      <c r="F2" s="65" t="s">
+        <v>146</v>
+      </c>
+      <c r="G2" s="85" t="s">
+        <v>666</v>
+      </c>
+      <c r="H2" s="57" t="s">
+        <v>460</v>
+      </c>
+      <c r="I2" s="57" t="s">
+        <v>361</v>
+      </c>
+      <c r="J2" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="K2" s="105" t="s">
+        <v>455</v>
+      </c>
+      <c r="L2" s="105" t="s">
+        <v>667</v>
+      </c>
+      <c r="M2" s="105" t="s">
+        <v>668</v>
+      </c>
+      <c r="N2" s="106" t="s">
+        <v>669</v>
+      </c>
+      <c r="O2" s="106"/>
+      <c r="P2" s="106" t="s">
+        <v>637</v>
+      </c>
+      <c r="Q2" s="105" t="s">
+        <v>670</v>
+      </c>
+      <c r="R2" s="106"/>
+      <c r="S2" s="106"/>
+      <c r="T2" s="106" t="s">
+        <v>639</v>
+      </c>
+      <c r="U2" s="105" t="s">
+        <v>455</v>
+      </c>
+      <c r="V2" s="105" t="s">
+        <v>455</v>
+      </c>
+      <c r="W2" s="105" t="s">
+        <v>455</v>
+      </c>
+      <c r="X2" s="105" t="s">
+        <v>455</v>
+      </c>
+      <c r="Y2" s="105" t="s">
+        <v>671</v>
+      </c>
+      <c r="Z2" s="86" t="s">
+        <v>641</v>
+      </c>
+      <c r="AA2" s="105" t="s">
+        <v>672</v>
+      </c>
+      <c r="AB2" s="57" t="s">
+        <v>642</v>
+      </c>
+      <c r="AC2" s="106" t="s">
+        <v>673</v>
+      </c>
+      <c r="AD2" s="105" t="s">
+        <v>671</v>
+      </c>
+      <c r="AE2" s="107"/>
+      <c r="AF2" s="48" t="s">
+        <v>669</v>
+      </c>
       <c r="AG2" s="57"/>
       <c r="AH2" s="57"/>
       <c r="AI2" s="57"/>

</xml_diff>

<commit_message>
GDE-9518: pulled dataset from repo and updated my changes.
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_ATM_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_ATM_BILAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99085DDB-8492-4C61-A8C3-30F8189305FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A433DA-FFD6-4728-A8CB-421AB6D6E991}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="737" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="737" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -2332,7 +2332,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2355,6 +2355,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2363,7 +2376,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2491,9 +2504,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2539,9 +2549,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="4" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="16" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2588,6 +2595,19 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2917,95 +2937,95 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" style="89" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25" style="89" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15" style="89" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="16.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="28.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="21.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="34.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="23.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="13.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="40" max="44" width="5.5703125" style="89" customWidth="1"/>
-    <col min="45" max="45" width="14.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="6.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="17.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="32.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="24.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="18.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="12.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="11.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="20.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="18.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="29.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="19" style="89" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="17.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="12.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="19.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="32.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="25.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="25.28515625" style="89" customWidth="1"/>
-    <col min="64" max="64" width="24.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="20.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="28" style="89" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="22.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="24.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="22.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="22.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="21" style="89" bestFit="1" customWidth="1"/>
-    <col min="72" max="73" width="23.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="32.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="32.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="29.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="17.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="22.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="21.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="21" style="89" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="22.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="24" style="89" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="26.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="26.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="23.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="21.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="35.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="35.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="32.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="22.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="15.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="18.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="30.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="27.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="20.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="29.85546875" style="89" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="86" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25" style="86" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15" style="86" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="16.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="28.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="34.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="23.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="40" max="44" width="5.5703125" style="86" customWidth="1"/>
+    <col min="45" max="45" width="14.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="6.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="17.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="32.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="24.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="18.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="12.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="11.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="20.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="18.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="29.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="19" style="86" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="17.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="12.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="19.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="32.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="25.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="25.28515625" style="86" customWidth="1"/>
+    <col min="64" max="64" width="24.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="20.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="28" style="86" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="22.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="24.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="22.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="22.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="21" style="86" bestFit="1" customWidth="1"/>
+    <col min="72" max="73" width="23.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="32.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="32.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="29.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="17.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="22.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="21.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="21" style="86" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="22.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="24" style="86" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="26.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="26.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="23.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="21.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="35.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="35.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="32.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="22.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="15.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="18.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="30.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="27.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="20.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="29.85546875" style="86" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:107" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3313,16 +3333,16 @@
       <c r="A2" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="85" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="88" t="s">
+      <c r="C2" s="85" t="s">
         <v>96</v>
       </c>
       <c r="D2" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="E2" s="88" t="s">
+      <c r="E2" s="85" t="s">
         <v>98</v>
       </c>
       <c r="F2" s="58" t="s">
@@ -3399,10 +3419,10 @@
       <c r="AG2" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="AH2" s="88" t="s">
+      <c r="AH2" s="85" t="s">
         <v>114</v>
       </c>
-      <c r="AI2" s="88" t="s">
+      <c r="AI2" s="85" t="s">
         <v>103</v>
       </c>
       <c r="AJ2" s="6"/>
@@ -3417,162 +3437,162 @@
       <c r="AS2" s="7"/>
       <c r="AT2" s="5"/>
       <c r="AU2" s="5"/>
-      <c r="AV2" s="88" t="s">
+      <c r="AV2" s="85" t="s">
         <v>115</v>
       </c>
-      <c r="AW2" s="88" t="s">
+      <c r="AW2" s="85" t="s">
         <v>116</v>
       </c>
       <c r="AX2" s="49"/>
       <c r="AY2" s="49"/>
       <c r="AZ2" s="49"/>
       <c r="BA2" s="49"/>
-      <c r="BB2" s="88" t="s">
+      <c r="BB2" s="85" t="s">
         <v>117</v>
       </c>
       <c r="BC2" s="49"/>
-      <c r="BD2" s="88" t="s">
+      <c r="BD2" s="85" t="s">
         <v>118</v>
       </c>
-      <c r="BE2" s="88" t="s">
+      <c r="BE2" s="85" t="s">
         <v>119</v>
       </c>
-      <c r="BF2" s="88" t="s">
+      <c r="BF2" s="85" t="s">
         <v>120</v>
       </c>
-      <c r="BG2" s="88" t="s">
+      <c r="BG2" s="85" t="s">
         <v>121</v>
       </c>
       <c r="BH2" s="64" t="s">
         <v>122</v>
       </c>
-      <c r="BI2" s="88" t="s">
+      <c r="BI2" s="85" t="s">
         <v>115</v>
       </c>
-      <c r="BJ2" s="88" t="s">
+      <c r="BJ2" s="85" t="s">
         <v>116</v>
       </c>
-      <c r="BK2" s="88"/>
-      <c r="BL2" s="88" t="s">
+      <c r="BK2" s="85"/>
+      <c r="BL2" s="85" t="s">
         <v>123</v>
       </c>
-      <c r="BM2" s="88" t="s">
+      <c r="BM2" s="85" t="s">
         <v>124</v>
       </c>
-      <c r="BN2" s="88" t="s">
+      <c r="BN2" s="85" t="s">
         <v>125</v>
       </c>
       <c r="BO2" s="49"/>
       <c r="BP2" s="49"/>
-      <c r="BQ2" s="88" t="s">
+      <c r="BQ2" s="85" t="s">
         <v>126</v>
       </c>
-      <c r="BR2" s="88" t="s">
+      <c r="BR2" s="85" t="s">
         <v>127</v>
       </c>
       <c r="BS2" s="65" t="s">
         <v>128</v>
       </c>
-      <c r="BT2" s="88" t="s">
+      <c r="BT2" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="BU2" s="88" t="s">
+      <c r="BU2" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="BV2" s="88" t="s">
+      <c r="BV2" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="BW2" s="88" t="s">
+      <c r="BW2" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="BX2" s="88" t="s">
+      <c r="BX2" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="BY2" s="88" t="s">
+      <c r="BY2" s="85" t="s">
         <v>107</v>
       </c>
-      <c r="BZ2" s="88" t="s">
+      <c r="BZ2" s="85" t="s">
         <v>130</v>
       </c>
-      <c r="CA2" s="88" t="s">
+      <c r="CA2" s="85" t="s">
         <v>131</v>
       </c>
-      <c r="CB2" s="88" t="s">
+      <c r="CB2" s="85" t="s">
         <v>132</v>
       </c>
-      <c r="CC2" s="88" t="s">
+      <c r="CC2" s="85" t="s">
         <v>133</v>
       </c>
-      <c r="CD2" s="88" t="s">
+      <c r="CD2" s="85" t="s">
         <v>134</v>
       </c>
-      <c r="CE2" s="88" t="s">
+      <c r="CE2" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="CF2" s="88" t="s">
+      <c r="CF2" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="CG2" s="88" t="s">
+      <c r="CG2" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="CH2" s="88" t="s">
+      <c r="CH2" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="CI2" s="88" t="s">
+      <c r="CI2" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="CJ2" s="88" t="s">
+      <c r="CJ2" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="CK2" s="88" t="s">
+      <c r="CK2" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="CL2" s="88" t="s">
+      <c r="CL2" s="85" t="s">
         <v>135</v>
       </c>
-      <c r="CM2" s="88" t="s">
+      <c r="CM2" s="85" t="s">
         <v>136</v>
       </c>
-      <c r="CN2" s="88" t="s">
+      <c r="CN2" s="85" t="s">
         <v>137</v>
       </c>
-      <c r="CO2" s="88" t="s">
+      <c r="CO2" s="85" t="s">
         <v>138</v>
       </c>
-      <c r="CP2" s="88" t="s">
+      <c r="CP2" s="85" t="s">
         <v>139</v>
       </c>
-      <c r="CQ2" s="88" t="s">
+      <c r="CQ2" s="85" t="s">
         <v>136</v>
       </c>
-      <c r="CR2" s="88" t="s">
+      <c r="CR2" s="85" t="s">
         <v>135</v>
       </c>
-      <c r="CS2" s="88"/>
-      <c r="CT2" s="88"/>
-      <c r="CU2" s="88"/>
-      <c r="CV2" s="88"/>
-      <c r="CW2" s="88"/>
-      <c r="CX2" s="88"/>
-      <c r="CY2" s="88"/>
-      <c r="CZ2" s="88"/>
-      <c r="DA2" s="88"/>
-      <c r="DB2" s="88"/>
+      <c r="CS2" s="85"/>
+      <c r="CT2" s="85"/>
+      <c r="CU2" s="85"/>
+      <c r="CV2" s="85"/>
+      <c r="CW2" s="85"/>
+      <c r="CX2" s="85"/>
+      <c r="CY2" s="85"/>
+      <c r="CZ2" s="85"/>
+      <c r="DA2" s="85"/>
+      <c r="DB2" s="85"/>
     </row>
     <row r="3" spans="1:107" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="85" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="85" t="s">
         <v>142</v>
       </c>
       <c r="D3" s="68" t="s">
         <v>143</v>
       </c>
-      <c r="E3" s="88" t="s">
+      <c r="E3" s="85" t="s">
         <v>144</v>
       </c>
       <c r="F3" s="58" t="s">
@@ -3649,10 +3669,10 @@
       <c r="AG3" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="AH3" s="88" t="s">
+      <c r="AH3" s="85" t="s">
         <v>114</v>
       </c>
-      <c r="AI3" s="88" t="s">
+      <c r="AI3" s="85" t="s">
         <v>103</v>
       </c>
       <c r="AJ3" s="6"/>
@@ -3667,137 +3687,137 @@
       <c r="AS3" s="7"/>
       <c r="AT3" s="5"/>
       <c r="AU3" s="5"/>
-      <c r="AV3" s="88" t="s">
+      <c r="AV3" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="AW3" s="88" t="s">
+      <c r="AW3" s="85" t="s">
         <v>146</v>
       </c>
       <c r="AX3" s="49"/>
       <c r="AY3" s="49"/>
       <c r="AZ3" s="49"/>
       <c r="BA3" s="49"/>
-      <c r="BB3" s="88" t="s">
+      <c r="BB3" s="85" t="s">
         <v>117</v>
       </c>
       <c r="BC3" s="49"/>
-      <c r="BD3" s="88" t="s">
+      <c r="BD3" s="85" t="s">
         <v>118</v>
       </c>
-      <c r="BE3" s="88" t="s">
+      <c r="BE3" s="85" t="s">
         <v>119</v>
       </c>
-      <c r="BF3" s="88" t="s">
+      <c r="BF3" s="85" t="s">
         <v>120</v>
       </c>
-      <c r="BG3" s="88" t="s">
+      <c r="BG3" s="85" t="s">
         <v>121</v>
       </c>
       <c r="BH3" s="64" t="s">
         <v>122</v>
       </c>
-      <c r="BI3" s="88" t="s">
+      <c r="BI3" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="BJ3" s="88" t="s">
+      <c r="BJ3" s="85" t="s">
         <v>146</v>
       </c>
       <c r="BK3" s="82">
         <v>60003007</v>
       </c>
-      <c r="BL3" s="88" t="s">
+      <c r="BL3" s="85" t="s">
         <v>147</v>
       </c>
-      <c r="BM3" s="88" t="s">
+      <c r="BM3" s="85" t="s">
         <v>124</v>
       </c>
-      <c r="BN3" s="88" t="s">
+      <c r="BN3" s="85" t="s">
         <v>125</v>
       </c>
       <c r="BO3" s="49"/>
       <c r="BP3" s="49"/>
-      <c r="BQ3" s="88" t="s">
+      <c r="BQ3" s="85" t="s">
         <v>126</v>
       </c>
-      <c r="BR3" s="88" t="s">
+      <c r="BR3" s="85" t="s">
         <v>127</v>
       </c>
       <c r="BS3" s="65" t="s">
         <v>128</v>
       </c>
-      <c r="BT3" s="88" t="s">
+      <c r="BT3" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="BU3" s="88" t="s">
+      <c r="BU3" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="BV3" s="88" t="s">
+      <c r="BV3" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="BW3" s="88" t="s">
+      <c r="BW3" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="BX3" s="88" t="s">
+      <c r="BX3" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="BY3" s="88" t="s">
+      <c r="BY3" s="85" t="s">
         <v>107</v>
       </c>
-      <c r="BZ3" s="88" t="s">
+      <c r="BZ3" s="85" t="s">
         <v>130</v>
       </c>
-      <c r="CA3" s="88" t="s">
+      <c r="CA3" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="CB3" s="88" t="s">
+      <c r="CB3" s="85" t="s">
         <v>149</v>
       </c>
-      <c r="CC3" s="88" t="s">
+      <c r="CC3" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="CD3" s="88" t="s">
+      <c r="CD3" s="85" t="s">
         <v>134</v>
       </c>
-      <c r="CE3" s="88" t="s">
+      <c r="CE3" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="CF3" s="88" t="s">
+      <c r="CF3" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="CG3" s="88" t="s">
+      <c r="CG3" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="CH3" s="88" t="s">
+      <c r="CH3" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="CI3" s="88" t="s">
+      <c r="CI3" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="CJ3" s="88" t="s">
+      <c r="CJ3" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="CK3" s="88" t="s">
+      <c r="CK3" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="CL3" s="88" t="s">
+      <c r="CL3" s="85" t="s">
         <v>135</v>
       </c>
-      <c r="CM3" s="88" t="s">
+      <c r="CM3" s="85" t="s">
         <v>136</v>
       </c>
-      <c r="CN3" s="88" t="s">
+      <c r="CN3" s="85" t="s">
         <v>151</v>
       </c>
-      <c r="CO3" s="88" t="s">
+      <c r="CO3" s="85" t="s">
         <v>152</v>
       </c>
-      <c r="CP3" s="88" t="s">
+      <c r="CP3" s="85" t="s">
         <v>139</v>
       </c>
-      <c r="CQ3" s="88" t="s">
+      <c r="CQ3" s="85" t="s">
         <v>136</v>
       </c>
-      <c r="CR3" s="88" t="s">
+      <c r="CR3" s="85" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3824,46 +3844,46 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="89" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="31.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12" style="89" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="30" style="89" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="32.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="31.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="24" style="89" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="25.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="24.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.42578125" style="89" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="86" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12" style="86" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="30" style="86" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="32.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="31.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24" style="86" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="25.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="24.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.42578125" style="86" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="107" t="s">
+      <c r="C1" s="101" t="s">
         <v>258</v>
       </c>
-      <c r="D1" s="106" t="s">
+      <c r="D1" s="100" t="s">
         <v>658</v>
       </c>
       <c r="E1" s="38" t="s">
@@ -3872,67 +3892,67 @@
       <c r="F1" s="38" t="s">
         <v>261</v>
       </c>
-      <c r="G1" s="107" t="s">
+      <c r="G1" s="101" t="s">
         <v>659</v>
       </c>
-      <c r="H1" s="107" t="s">
+      <c r="H1" s="101" t="s">
         <v>660</v>
       </c>
-      <c r="I1" s="109" t="s">
+      <c r="I1" s="103" t="s">
         <v>661</v>
       </c>
-      <c r="J1" s="108" t="s">
+      <c r="J1" s="102" t="s">
         <v>662</v>
       </c>
-      <c r="K1" s="108" t="s">
+      <c r="K1" s="102" t="s">
         <v>619</v>
       </c>
-      <c r="L1" s="108" t="s">
+      <c r="L1" s="102" t="s">
         <v>663</v>
       </c>
-      <c r="M1" s="106" t="s">
+      <c r="M1" s="100" t="s">
         <v>664</v>
       </c>
-      <c r="N1" s="106" t="s">
+      <c r="N1" s="100" t="s">
         <v>665</v>
       </c>
-      <c r="O1" s="106" t="s">
+      <c r="O1" s="100" t="s">
         <v>617</v>
       </c>
-      <c r="P1" s="106" t="s">
+      <c r="P1" s="100" t="s">
         <v>666</v>
       </c>
-      <c r="Q1" s="110" t="s">
+      <c r="Q1" s="104" t="s">
         <v>628</v>
       </c>
-      <c r="R1" s="106" t="s">
+      <c r="R1" s="100" t="s">
         <v>667</v>
       </c>
-      <c r="S1" s="117" t="s">
+      <c r="S1" s="111" t="s">
         <v>668</v>
       </c>
-      <c r="T1" s="117" t="s">
+      <c r="T1" s="111" t="s">
         <v>669</v>
       </c>
-      <c r="U1" s="117" t="s">
+      <c r="U1" s="111" t="s">
         <v>670</v>
       </c>
-      <c r="V1" s="117" t="s">
+      <c r="V1" s="111" t="s">
         <v>671</v>
       </c>
-      <c r="W1" s="118" t="s">
+      <c r="W1" s="112" t="s">
         <v>672</v>
       </c>
-      <c r="X1" s="118" t="s">
+      <c r="X1" s="112" t="s">
         <v>673</v>
       </c>
-      <c r="Y1" s="118" t="s">
+      <c r="Y1" s="112" t="s">
         <v>674</v>
       </c>
-      <c r="Z1" s="118" t="s">
+      <c r="Z1" s="112" t="s">
         <v>675</v>
       </c>
-      <c r="AA1" s="118" t="s">
+      <c r="AA1" s="112" t="s">
         <v>676</v>
       </c>
     </row>
@@ -3940,135 +3960,135 @@
       <c r="A2" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="105" t="s">
         <v>677</v>
       </c>
-      <c r="C2" s="88" t="s">
+      <c r="C2" s="85" t="s">
         <v>700</v>
       </c>
-      <c r="D2" s="112" t="s">
+      <c r="D2" s="106" t="s">
         <v>460</v>
       </c>
-      <c r="E2" s="88" t="s">
+      <c r="E2" s="85" t="s">
         <v>350</v>
       </c>
-      <c r="F2" s="88" t="s">
+      <c r="F2" s="85" t="s">
         <v>351</v>
       </c>
-      <c r="G2" s="111" t="s">
+      <c r="G2" s="105" t="s">
         <v>678</v>
       </c>
-      <c r="H2" s="111"/>
-      <c r="I2" s="88" t="s">
+      <c r="H2" s="105"/>
+      <c r="I2" s="85" t="s">
         <v>146</v>
       </c>
-      <c r="J2" s="113">
+      <c r="J2" s="107">
         <v>61621757</v>
       </c>
-      <c r="K2" s="113">
+      <c r="K2" s="107">
         <v>61621757</v>
       </c>
-      <c r="L2" s="111"/>
-      <c r="M2" s="112" t="s">
+      <c r="L2" s="105"/>
+      <c r="M2" s="106" t="s">
         <v>679</v>
       </c>
-      <c r="N2" s="112" t="s">
+      <c r="N2" s="106" t="s">
         <v>680</v>
       </c>
-      <c r="O2" s="112" t="s">
+      <c r="O2" s="106" t="s">
         <v>361</v>
       </c>
-      <c r="P2" s="114" t="s">
+      <c r="P2" s="108" t="s">
         <v>643</v>
       </c>
-      <c r="Q2" s="111" t="s">
+      <c r="Q2" s="105" t="s">
         <v>646</v>
       </c>
-      <c r="R2" s="114"/>
-      <c r="S2" s="123"/>
-      <c r="T2" s="123"/>
-      <c r="U2" s="123"/>
-      <c r="V2" s="123"/>
-      <c r="W2" s="123"/>
-      <c r="X2" s="123"/>
-      <c r="Y2" s="123"/>
-      <c r="Z2" s="123"/>
-      <c r="AA2" s="123"/>
+      <c r="R2" s="108"/>
+      <c r="S2" s="117"/>
+      <c r="T2" s="117"/>
+      <c r="U2" s="117"/>
+      <c r="V2" s="117"/>
+      <c r="W2" s="117"/>
+      <c r="X2" s="117"/>
+      <c r="Y2" s="117"/>
+      <c r="Z2" s="117"/>
+      <c r="AA2" s="117"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="115" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="93" t="s">
         <v>681</v>
       </c>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="85" t="s">
         <v>348</v>
       </c>
-      <c r="D3" s="115" t="s">
+      <c r="D3" s="109" t="s">
         <v>460</v>
       </c>
-      <c r="E3" s="122" t="s">
+      <c r="E3" s="116" t="s">
         <v>350</v>
       </c>
-      <c r="F3" s="122" t="s">
+      <c r="F3" s="116" t="s">
         <v>351</v>
       </c>
-      <c r="G3" s="111" t="s">
+      <c r="G3" s="105" t="s">
         <v>682</v>
       </c>
-      <c r="H3" s="123"/>
-      <c r="I3" s="122" t="s">
+      <c r="H3" s="117"/>
+      <c r="I3" s="116" t="s">
         <v>116</v>
       </c>
-      <c r="J3" s="98" t="s">
+      <c r="J3" s="95" t="s">
         <v>456</v>
       </c>
-      <c r="K3" s="98" t="s">
+      <c r="K3" s="95" t="s">
         <v>456</v>
       </c>
-      <c r="L3" s="123"/>
-      <c r="M3" s="115" t="s">
+      <c r="L3" s="117"/>
+      <c r="M3" s="109" t="s">
         <v>679</v>
       </c>
-      <c r="N3" s="115" t="s">
+      <c r="N3" s="109" t="s">
         <v>680</v>
       </c>
-      <c r="O3" s="115" t="s">
+      <c r="O3" s="109" t="s">
         <v>361</v>
       </c>
-      <c r="P3" s="116" t="s">
+      <c r="P3" s="110" t="s">
         <v>683</v>
       </c>
-      <c r="Q3" s="111" t="s">
+      <c r="Q3" s="105" t="s">
         <v>646</v>
       </c>
-      <c r="R3" s="123"/>
-      <c r="S3" s="119" t="s">
+      <c r="R3" s="117"/>
+      <c r="S3" s="113" t="s">
         <v>684</v>
       </c>
-      <c r="T3" s="119" t="s">
+      <c r="T3" s="113" t="s">
         <v>684</v>
       </c>
-      <c r="U3" s="119" t="s">
+      <c r="U3" s="113" t="s">
         <v>684</v>
       </c>
-      <c r="V3" s="119" t="s">
+      <c r="V3" s="113" t="s">
         <v>685</v>
       </c>
-      <c r="W3" s="119" t="s">
+      <c r="W3" s="113" t="s">
         <v>655</v>
       </c>
-      <c r="X3" s="119" t="s">
+      <c r="X3" s="113" t="s">
         <v>459</v>
       </c>
-      <c r="Y3" s="120" t="s">
+      <c r="Y3" s="114" t="s">
         <v>650</v>
       </c>
-      <c r="Z3" s="120" t="s">
+      <c r="Z3" s="114" t="s">
         <v>591</v>
       </c>
-      <c r="AA3" s="120" t="s">
+      <c r="AA3" s="114" t="s">
         <v>644</v>
       </c>
     </row>
@@ -4090,124 +4110,124 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="95" customWidth="1"/>
-    <col min="2" max="2" width="51" style="95" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" style="95" customWidth="1"/>
-    <col min="4" max="4" width="38.28515625" style="95" customWidth="1"/>
-    <col min="5" max="6" width="41" style="95" customWidth="1"/>
-    <col min="7" max="7" width="25" style="95" customWidth="1"/>
-    <col min="8" max="8" width="28" style="95" customWidth="1"/>
-    <col min="9" max="9" width="37" style="95" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="26.28515625" style="95" customWidth="1"/>
-    <col min="14" max="14" width="22" style="95" customWidth="1"/>
-    <col min="15" max="15" width="30.28515625" style="95" customWidth="1"/>
-    <col min="16" max="30" width="9.140625" style="95" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="95"/>
+    <col min="1" max="1" width="9.140625" style="92" customWidth="1"/>
+    <col min="2" max="2" width="51" style="92" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="92" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" style="92" customWidth="1"/>
+    <col min="5" max="6" width="41" style="92" customWidth="1"/>
+    <col min="7" max="7" width="25" style="92" customWidth="1"/>
+    <col min="8" max="8" width="28" style="92" customWidth="1"/>
+    <col min="9" max="9" width="37" style="92" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="26.28515625" style="92" customWidth="1"/>
+    <col min="14" max="14" width="22" style="92" customWidth="1"/>
+    <col min="15" max="15" width="30.28515625" style="92" customWidth="1"/>
+    <col min="16" max="30" width="9.140625" style="92" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="92"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="92" t="s">
+      <c r="C1" s="89" t="s">
         <v>558</v>
       </c>
-      <c r="D1" s="92" t="s">
+      <c r="D1" s="89" t="s">
         <v>686</v>
       </c>
-      <c r="E1" s="92" t="s">
+      <c r="E1" s="89" t="s">
         <v>687</v>
       </c>
-      <c r="F1" s="92" t="s">
+      <c r="F1" s="89" t="s">
         <v>688</v>
       </c>
-      <c r="G1" s="92" t="s">
+      <c r="G1" s="89" t="s">
         <v>689</v>
       </c>
-      <c r="H1" s="92" t="s">
+      <c r="H1" s="89" t="s">
         <v>619</v>
       </c>
-      <c r="I1" s="92" t="s">
+      <c r="I1" s="89" t="s">
         <v>690</v>
       </c>
-      <c r="J1" s="93" t="s">
+      <c r="J1" s="90" t="s">
         <v>691</v>
       </c>
-      <c r="K1" s="93" t="s">
+      <c r="K1" s="90" t="s">
         <v>544</v>
       </c>
-      <c r="L1" s="93" t="s">
+      <c r="L1" s="90" t="s">
         <v>692</v>
       </c>
-      <c r="M1" s="93" t="s">
+      <c r="M1" s="90" t="s">
         <v>617</v>
       </c>
-      <c r="N1" s="94" t="s">
+      <c r="N1" s="91" t="s">
         <v>560</v>
       </c>
-      <c r="O1" s="94" t="s">
+      <c r="O1" s="91" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="93" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="93" t="s">
         <v>693</v>
       </c>
-      <c r="C2" s="96" t="s">
+      <c r="C2" s="93" t="s">
         <v>694</v>
       </c>
-      <c r="D2" s="96" t="s">
+      <c r="D2" s="93" t="s">
         <v>695</v>
       </c>
-      <c r="E2" s="97" t="s">
+      <c r="E2" s="94" t="s">
         <v>696</v>
       </c>
-      <c r="F2" s="97" t="s">
+      <c r="F2" s="94" t="s">
         <v>697</v>
       </c>
-      <c r="G2" s="97" t="s">
+      <c r="G2" s="94" t="s">
         <v>697</v>
       </c>
-      <c r="H2" s="98" t="s">
+      <c r="H2" s="95" t="s">
         <v>543</v>
       </c>
-      <c r="I2" s="98" t="s">
+      <c r="I2" s="95" t="s">
         <v>698</v>
       </c>
-      <c r="J2" s="98" t="s">
+      <c r="J2" s="95" t="s">
         <v>585</v>
       </c>
-      <c r="K2" s="98" t="s">
+      <c r="K2" s="95" t="s">
         <v>548</v>
       </c>
-      <c r="L2" s="102" t="s">
+      <c r="L2" s="99" t="s">
         <v>699</v>
       </c>
-      <c r="M2" s="97" t="s">
+      <c r="M2" s="94" t="s">
         <v>472</v>
       </c>
-      <c r="N2" s="96" t="s">
+      <c r="N2" s="93" t="s">
         <v>139</v>
       </c>
-      <c r="O2" s="96" t="s">
+      <c r="O2" s="93" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="L9" s="99"/>
-      <c r="M9" s="99"/>
+      <c r="L9" s="96"/>
+      <c r="M9" s="96"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J10" s="100"/>
-      <c r="K10" s="100"/>
-      <c r="L10" s="100"/>
-      <c r="M10" s="100"/>
+      <c r="J10" s="97"/>
+      <c r="K10" s="97"/>
+      <c r="L10" s="97"/>
+      <c r="M10" s="97"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4227,134 +4247,134 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="17.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22" style="89" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16" style="89" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19" style="89" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.85546875" style="89" customWidth="1"/>
-    <col min="19" max="19" width="24.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="26.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="29" style="89" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24" style="89" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="23.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="32.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="32.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="29.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="47.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="48.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="47" style="89" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="48" style="89" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="48.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="49.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="41.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="43" style="89" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="41.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="35.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="43.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="44.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="41" style="89" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="42.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="42.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="18.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="15.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="18" style="89" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="23" style="89" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="16" style="89" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="24.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="26.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="29.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="56" max="57" width="54.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="36.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="19" style="89" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="21" style="89" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="36.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="20.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="10.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="28" style="89" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="22.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="25" style="89" bestFit="1" customWidth="1"/>
-    <col min="67" max="68" width="35.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="34.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="40.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="42.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="39.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="33.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="41.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="42.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="39.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="19.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="19.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="35.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="40.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="40.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="34.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="39.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="45.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="49.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="36.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="12.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="24" style="89" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="19.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="20.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="25.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="20.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="26.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="20.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="25.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="20.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="22.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="98" max="99" width="22.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="29.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="21.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="19" style="89" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="16.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="21.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="12.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="16.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="21" style="89" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="21.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="19" style="89" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="20.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="19" style="89" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="29.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="20" style="89" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="29.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="20.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="31.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="29.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="28.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="26.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="26.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="23.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="21.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="24.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="22.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="35.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="35.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="32.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="22.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="37.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="130" max="130" width="23.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="131" max="131" width="18.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="18.28515625" style="89" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="17.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22" style="86" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16" style="86" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19" style="86" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.85546875" style="86" customWidth="1"/>
+    <col min="19" max="19" width="24.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29" style="86" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24" style="86" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="32.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="32.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="29.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="47.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="48.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="47" style="86" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="48" style="86" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="48.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="49.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="41.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="43" style="86" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="41.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="35.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="43.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="44.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="41" style="86" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="42.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="42.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="18.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="15.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18" style="86" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="23" style="86" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="16" style="86" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="24.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="26.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="29.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="56" max="57" width="54.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="36.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="19" style="86" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="21" style="86" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="36.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="20.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="10.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="28" style="86" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="22.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="25" style="86" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="35.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="34.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="40.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="42.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="39.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="33.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="41.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="42.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="39.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="19.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="19.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="35.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="40.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="40.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="34.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="39.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="45.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="49.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="36.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="12.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="24" style="86" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="19.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="20.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="25.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="20.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="26.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="20.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="25.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="20.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="22.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="98" max="99" width="22.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="29.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="21.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="19" style="86" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="16.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="21.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="12.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="16.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="21" style="86" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="21.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="19" style="86" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="20.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="19" style="86" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="29.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="20" style="86" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="29.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="20.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="31.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="29.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="28.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="26.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="26.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="23.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="21.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="24.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="22.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="35.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="35.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="32.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="22.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="37.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="130" max="130" width="23.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="18.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="18.28515625" style="86" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:135" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4765,10 +4785,10 @@
       </c>
     </row>
     <row r="2" spans="1:135" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="85" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="88"/>
+      <c r="B2" s="85"/>
       <c r="C2" s="17" t="s">
         <v>115</v>
       </c>
@@ -4790,7 +4810,7 @@
       <c r="O2" s="35"/>
       <c r="P2" s="16"/>
       <c r="Q2" s="16"/>
-      <c r="R2" s="88" t="s">
+      <c r="R2" s="85" t="s">
         <v>137</v>
       </c>
       <c r="S2" s="19"/>
@@ -4949,98 +4969,98 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" style="89" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.85546875" style="89" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" style="89" customWidth="1"/>
-    <col min="15" max="15" width="28.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="36.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="44.42578125" style="89" customWidth="1"/>
-    <col min="21" max="21" width="22" style="89" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="27.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23" style="89" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="21" style="89" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="22.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="25" style="89" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="24.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="41.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="42.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="21" style="89" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="44.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="26.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="36.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="35.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="47.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="40.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="26.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="40.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="31.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="26" style="89" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="26.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="16.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="34.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="28.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="17.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="55" max="56" width="15.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="20.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="16.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="9.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="13.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="16" style="89" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="17.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="20.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="16.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="21.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="18.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="36.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="18.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="27.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="22.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="19" style="89" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="26.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="24" style="89" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="28.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="26.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="24" style="89" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="19.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="24" style="89" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="21.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="36.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="29.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="24.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="24.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="21.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="26" style="89" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="22" style="89" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="20.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="30.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="31.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="17" style="89" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="28.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="32.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="30.5703125" style="89" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" style="86" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.85546875" style="86" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" style="86" customWidth="1"/>
+    <col min="15" max="15" width="28.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="36.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="44.42578125" style="86" customWidth="1"/>
+    <col min="21" max="21" width="22" style="86" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23" style="86" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="21" style="86" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="25" style="86" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="24.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="41.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="42.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="21" style="86" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="44.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="26.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="36.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="35.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="47.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="40.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="26.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="40.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="31.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="26" style="86" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="26.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="16.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="34.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="28.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="17.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="55" max="56" width="15.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="20.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="16.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="9.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="13.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="16" style="86" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="17.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="20.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="16.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="21.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="18.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="36.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="18.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="27.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="22.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="19" style="86" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="26.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="24" style="86" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="28.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="26.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="24" style="86" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="19.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="24" style="86" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="21.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="36.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="29.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="24.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="24.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="21.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="26" style="86" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="22" style="86" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="20.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="30.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="31.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="17" style="86" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="28.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="32.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="30.5703125" style="86" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:96" s="56" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5337,47 +5357,47 @@
       <c r="A2" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="85" t="s">
         <v>345</v>
       </c>
-      <c r="C2" s="88" t="s">
+      <c r="C2" s="85" t="s">
         <v>346</v>
       </c>
-      <c r="D2" s="88" t="s">
+      <c r="D2" s="85" t="s">
         <v>347</v>
       </c>
-      <c r="E2" s="88" t="s">
+      <c r="E2" s="85" t="s">
         <v>348</v>
       </c>
-      <c r="F2" s="88" t="s">
+      <c r="F2" s="85" t="s">
         <v>349</v>
       </c>
-      <c r="G2" s="88" t="s">
+      <c r="G2" s="85" t="s">
         <v>350</v>
       </c>
-      <c r="H2" s="88" t="s">
+      <c r="H2" s="85" t="s">
         <v>351</v>
       </c>
-      <c r="I2" s="88" t="s">
+      <c r="I2" s="85" t="s">
         <v>134</v>
       </c>
-      <c r="J2" s="88" t="s">
+      <c r="J2" s="85" t="s">
         <v>116</v>
       </c>
-      <c r="K2" s="88" t="s">
+      <c r="K2" s="85" t="s">
         <v>146</v>
       </c>
-      <c r="L2" s="88"/>
+      <c r="L2" s="85"/>
       <c r="M2" s="62" t="s">
         <v>97</v>
       </c>
       <c r="N2" s="62" t="s">
         <v>143</v>
       </c>
-      <c r="O2" s="88" t="s">
+      <c r="O2" s="85" t="s">
         <v>135</v>
       </c>
-      <c r="P2" s="88" t="s">
+      <c r="P2" s="85" t="s">
         <v>137</v>
       </c>
       <c r="Q2" s="46" t="s">
@@ -5386,7 +5406,7 @@
       <c r="R2" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="S2" s="88" t="s">
+      <c r="S2" s="85" t="s">
         <v>139</v>
       </c>
       <c r="T2" s="23" t="s">
@@ -5407,10 +5427,10 @@
       <c r="Y2" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="Z2" s="88" t="s">
+      <c r="Z2" s="85" t="s">
         <v>355</v>
       </c>
-      <c r="AA2" s="88" t="s">
+      <c r="AA2" s="85" t="s">
         <v>356</v>
       </c>
       <c r="AB2" s="35" t="s">
@@ -5419,28 +5439,28 @@
       <c r="AC2" s="48"/>
       <c r="AD2" s="48"/>
       <c r="AE2" s="13"/>
-      <c r="AF2" s="88" t="s">
+      <c r="AF2" s="85" t="s">
         <v>120</v>
       </c>
-      <c r="AG2" s="88" t="s">
+      <c r="AG2" s="85" t="s">
         <v>358</v>
       </c>
-      <c r="AH2" s="88" t="s">
+      <c r="AH2" s="85" t="s">
         <v>119</v>
       </c>
-      <c r="AI2" s="88" t="s">
+      <c r="AI2" s="85" t="s">
         <v>359</v>
       </c>
-      <c r="AJ2" s="88" t="s">
+      <c r="AJ2" s="85" t="s">
         <v>360</v>
       </c>
-      <c r="AK2" s="88" t="s">
+      <c r="AK2" s="85" t="s">
         <v>361</v>
       </c>
-      <c r="AL2" s="88" t="s">
+      <c r="AL2" s="85" t="s">
         <v>362</v>
       </c>
-      <c r="AM2" s="88" t="s">
+      <c r="AM2" s="85" t="s">
         <v>362</v>
       </c>
       <c r="AN2" s="46" t="s">
@@ -5625,63 +5645,63 @@
   </sheetPr>
   <dimension ref="A1:BJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AU1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="AU1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="BA8" sqref="BA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" style="89" customWidth="1"/>
-    <col min="5" max="5" width="34.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" style="89" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" style="89" customWidth="1"/>
-    <col min="17" max="17" width="20.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="36.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="49.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="49.28515625" style="89" customWidth="1"/>
-    <col min="24" max="24" width="26" style="89" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="32" style="89" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="32.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="31" style="89" customWidth="1"/>
-    <col min="29" max="30" width="25.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="25" style="89" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="28" style="89" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="21" style="89" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="26.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="26.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="26.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="38" max="39" width="27.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="40" max="41" width="15.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="42" max="43" width="20.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="44" max="45" width="33.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="46" max="47" width="16.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="16.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="20.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="17.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="19.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="19.140625" style="89" customWidth="1"/>
-    <col min="53" max="53" width="20" style="89" bestFit="1" customWidth="1"/>
-    <col min="54" max="55" width="22.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="14.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="21.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="17.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="22.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="60" max="61" width="21.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="15.7109375" style="89" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" style="86" customWidth="1"/>
+    <col min="5" max="5" width="34.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" style="86" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" style="86" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="36.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="49.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="49.28515625" style="86" customWidth="1"/>
+    <col min="24" max="24" width="26" style="86" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="32" style="86" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="32.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="31" style="86" customWidth="1"/>
+    <col min="29" max="30" width="25.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="25" style="86" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="28" style="86" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="21" style="86" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="26.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="26.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="26.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="27.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="40" max="41" width="15.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="42" max="43" width="20.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="44" max="45" width="33.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="46" max="47" width="16.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="16.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="20.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="17.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="19.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="19.140625" style="86" customWidth="1"/>
+    <col min="53" max="53" width="20" style="86" bestFit="1" customWidth="1"/>
+    <col min="54" max="55" width="22.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="14.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="21.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="17.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="22.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="21.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="15.7109375" style="86" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:62" s="44" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -5876,7 +5896,7 @@
       <c r="A2" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="85" t="s">
         <v>345</v>
       </c>
       <c r="C2" s="46" t="s">
@@ -5885,7 +5905,7 @@
       <c r="D2" s="46" t="s">
         <v>351</v>
       </c>
-      <c r="E2" s="88" t="s">
+      <c r="E2" s="85" t="s">
         <v>348</v>
       </c>
       <c r="F2" s="46" t="s">
@@ -5924,7 +5944,7 @@
       <c r="Q2" s="35" t="s">
         <v>459</v>
       </c>
-      <c r="R2" s="88" t="s">
+      <c r="R2" s="85" t="s">
         <v>353</v>
       </c>
       <c r="S2" s="33" t="s">
@@ -5951,10 +5971,10 @@
       <c r="Z2" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="AA2" s="88" t="s">
+      <c r="AA2" s="85" t="s">
         <v>146</v>
       </c>
-      <c r="AB2" s="88" t="s">
+      <c r="AB2" s="85" t="s">
         <v>116</v>
       </c>
       <c r="AC2" s="46" t="s">
@@ -6041,13 +6061,13 @@
       <c r="BD2" s="77" t="s">
         <v>474</v>
       </c>
-      <c r="BE2" s="88" t="s">
+      <c r="BE2" s="85" t="s">
         <v>475</v>
       </c>
-      <c r="BF2" s="88" t="s">
+      <c r="BF2" s="85" t="s">
         <v>375</v>
       </c>
-      <c r="BG2" s="88" t="s">
+      <c r="BG2" s="85" t="s">
         <v>394</v>
       </c>
       <c r="BH2" s="43" t="s">
@@ -6079,48 +6099,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="29.85546875" style="89" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="27" style="89" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="27" style="89" customWidth="1"/>
-    <col min="15" max="15" width="29.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="18" max="21" width="28.140625" style="89" customWidth="1"/>
-    <col min="22" max="22" width="26" style="89" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="22.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="29.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="26.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="26.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="24.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="21.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="26.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="30.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="21.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="40" max="41" width="25.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="21" style="89" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="22" style="89" bestFit="1" customWidth="1"/>
-    <col min="44" max="45" width="26.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="15.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="48" max="49" width="14.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="23" style="89" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="18.5703125" style="89" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="29.85546875" style="86" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="27" style="86" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="27" style="86" customWidth="1"/>
+    <col min="15" max="15" width="29.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="18" max="21" width="28.140625" style="86" customWidth="1"/>
+    <col min="22" max="22" width="26" style="86" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="29.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="26.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="26.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="21.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="26.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="30.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="21.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="40" max="41" width="25.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="21" style="86" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="22" style="86" bestFit="1" customWidth="1"/>
+    <col min="44" max="45" width="26.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="15.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="48" max="49" width="14.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="23" style="86" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="18.5703125" style="86" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:51" s="37" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6259,22 +6279,22 @@
       <c r="AS1" s="37" t="s">
         <v>513</v>
       </c>
-      <c r="AT1" s="87" t="s">
+      <c r="AT1" s="84" t="s">
         <v>514</v>
       </c>
-      <c r="AU1" s="87" t="s">
+      <c r="AU1" s="84" t="s">
         <v>515</v>
       </c>
-      <c r="AV1" s="87" t="s">
+      <c r="AV1" s="84" t="s">
         <v>516</v>
       </c>
-      <c r="AW1" s="87" t="s">
+      <c r="AW1" s="84" t="s">
         <v>517</v>
       </c>
-      <c r="AX1" s="87" t="s">
+      <c r="AX1" s="84" t="s">
         <v>518</v>
       </c>
-      <c r="AY1" s="87" t="s">
+      <c r="AY1" s="84" t="s">
         <v>519</v>
       </c>
     </row>
@@ -6282,35 +6302,35 @@
       <c r="A2" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="85" t="s">
         <v>345</v>
       </c>
-      <c r="C2" s="88" t="s">
+      <c r="C2" s="85" t="s">
         <v>348</v>
       </c>
-      <c r="D2" s="88" t="s">
+      <c r="D2" s="85" t="s">
         <v>350</v>
       </c>
-      <c r="E2" s="88" t="s">
+      <c r="E2" s="85" t="s">
         <v>351</v>
       </c>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88" t="s">
+      <c r="F2" s="85"/>
+      <c r="G2" s="85" t="s">
         <v>475</v>
       </c>
-      <c r="H2" s="88" t="s">
+      <c r="H2" s="85" t="s">
         <v>375</v>
       </c>
-      <c r="I2" s="88" t="s">
+      <c r="I2" s="85" t="s">
         <v>375</v>
       </c>
-      <c r="J2" s="88" t="s">
+      <c r="J2" s="85" t="s">
         <v>394</v>
       </c>
-      <c r="K2" s="88" t="s">
+      <c r="K2" s="85" t="s">
         <v>520</v>
       </c>
-      <c r="L2" s="88" t="s">
+      <c r="L2" s="85" t="s">
         <v>521</v>
       </c>
       <c r="M2" s="46" t="s">
@@ -6322,7 +6342,7 @@
       <c r="O2" s="46" t="s">
         <v>522</v>
       </c>
-      <c r="P2" s="88" t="s">
+      <c r="P2" s="85" t="s">
         <v>524</v>
       </c>
       <c r="Q2" s="46" t="s">
@@ -6338,10 +6358,10 @@
         <v>525</v>
       </c>
       <c r="U2" s="46"/>
-      <c r="V2" s="88" t="s">
+      <c r="V2" s="85" t="s">
         <v>527</v>
       </c>
-      <c r="W2" s="88" t="s">
+      <c r="W2" s="85" t="s">
         <v>528</v>
       </c>
       <c r="X2" s="43" t="s">
@@ -6413,22 +6433,22 @@
       <c r="A3" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="83" t="s">
         <v>542</v>
       </c>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="85" t="s">
         <v>348</v>
       </c>
-      <c r="D3" s="88" t="s">
+      <c r="D3" s="85" t="s">
         <v>350</v>
       </c>
-      <c r="E3" s="88" t="s">
+      <c r="E3" s="85" t="s">
         <v>351</v>
       </c>
       <c r="AC3" s="43" t="s">
         <v>375</v>
       </c>
-      <c r="AT3" s="101" t="s">
+      <c r="AT3" s="98" t="s">
         <v>94</v>
       </c>
       <c r="AU3" s="46" t="s">
@@ -6440,15 +6460,15 @@
       <c r="AW3" s="46" t="s">
         <v>522</v>
       </c>
-      <c r="AX3" s="91" t="s">
+      <c r="AX3" s="88" t="s">
         <v>543</v>
       </c>
-      <c r="AY3" s="91" t="s">
+      <c r="AY3" s="88" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="4" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="C4" s="88" t="s">
+      <c r="C4" s="85" t="s">
         <v>348</v>
       </c>
       <c r="D4" t="s">
@@ -6459,7 +6479,7 @@
       </c>
     </row>
     <row r="5" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="C5" s="88" t="s">
+      <c r="C5" s="85" t="s">
         <v>348</v>
       </c>
       <c r="D5" t="s">
@@ -6470,7 +6490,7 @@
       </c>
     </row>
     <row r="6" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="C6" s="88" t="s">
+      <c r="C6" s="85" t="s">
         <v>348</v>
       </c>
       <c r="D6" t="s">
@@ -6481,7 +6501,7 @@
       </c>
     </row>
     <row r="7" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="C7" s="88" t="s">
+      <c r="C7" s="85" t="s">
         <v>348</v>
       </c>
       <c r="D7" t="s">
@@ -6564,12 +6584,12 @@
       <c r="B2" s="73" t="s">
         <v>345</v>
       </c>
-      <c r="C2" s="88" t="s">
+      <c r="C2" s="85" t="s">
         <v>348</v>
       </c>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88" t="s">
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85" t="s">
         <v>548</v>
       </c>
       <c r="G2" s="77" t="s">
@@ -6606,33 +6626,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26" style="89" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21" style="89" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="19.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="29.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="29.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9" style="89" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14" style="89" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18" style="89" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="16.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.42578125" style="89" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26" style="86" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" style="86" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="19.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="29.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9" style="86" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14" style="86" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18" style="86" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="16.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.42578125" style="86" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" s="44" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -6743,16 +6763,16 @@
       <c r="A2" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="85" t="s">
         <v>579</v>
       </c>
-      <c r="C2" s="88" t="s">
+      <c r="C2" s="85" t="s">
         <v>348</v>
       </c>
       <c r="D2" s="46" t="s">
         <v>375</v>
       </c>
-      <c r="E2" s="88"/>
+      <c r="E2" s="85"/>
       <c r="F2" s="46" t="s">
         <v>580</v>
       </c>
@@ -6858,30 +6878,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" style="89" customWidth="1"/>
-    <col min="6" max="6" width="36.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21" style="89" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" style="89" customWidth="1"/>
-    <col min="14" max="14" width="20.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="31.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25" style="89" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="34.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="34.85546875" style="89" customWidth="1"/>
-    <col min="23" max="23" width="27.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.42578125" style="89" customWidth="1"/>
-    <col min="25" max="25" width="18" style="89" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" style="86" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21" style="86" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" style="86" customWidth="1"/>
+    <col min="14" max="14" width="20.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="31.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25" style="86" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="34.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="34.85546875" style="86" customWidth="1"/>
+    <col min="23" max="23" width="27.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.42578125" style="86" customWidth="1"/>
+    <col min="25" max="25" width="18" style="86" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6973,16 +6993,16 @@
       <c r="A2" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="85" t="s">
         <v>345</v>
       </c>
-      <c r="C2" s="88" t="s">
+      <c r="C2" s="85" t="s">
         <v>348</v>
       </c>
-      <c r="D2" s="88" t="s">
+      <c r="D2" s="85" t="s">
         <v>350</v>
       </c>
-      <c r="E2" s="88" t="s">
+      <c r="E2" s="85" t="s">
         <v>351</v>
       </c>
       <c r="F2" s="39" t="s">
@@ -7021,19 +7041,19 @@
       <c r="Q2" s="57" t="s">
         <v>612</v>
       </c>
-      <c r="R2" s="88" t="s">
+      <c r="R2" s="85" t="s">
         <v>117</v>
       </c>
-      <c r="S2" s="88" t="s">
+      <c r="S2" s="85" t="s">
         <v>383</v>
       </c>
-      <c r="T2" s="88" t="s">
+      <c r="T2" s="85" t="s">
         <v>114</v>
       </c>
-      <c r="U2" s="88" t="s">
+      <c r="U2" s="85" t="s">
         <v>466</v>
       </c>
-      <c r="V2" s="88" t="s">
+      <c r="V2" s="85" t="s">
         <v>119</v>
       </c>
       <c r="W2" s="35" t="s">
@@ -7042,17 +7062,17 @@
       <c r="X2" s="57" t="s">
         <v>357</v>
       </c>
-      <c r="Y2" s="88" t="s">
+      <c r="Y2" s="85" t="s">
         <v>614</v>
       </c>
-      <c r="Z2" s="88"/>
-      <c r="AA2" s="88"/>
-      <c r="AB2" s="88"/>
-      <c r="AC2" s="88"/>
-      <c r="AD2" s="88"/>
-      <c r="AE2" s="88"/>
-      <c r="AF2" s="88"/>
-      <c r="AG2" s="88"/>
+      <c r="Z2" s="85"/>
+      <c r="AA2" s="85"/>
+      <c r="AB2" s="85"/>
+      <c r="AC2" s="85"/>
+      <c r="AD2" s="85"/>
+      <c r="AE2" s="85"/>
+      <c r="AF2" s="85"/>
+      <c r="AG2" s="85"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="Q3" t="s">
@@ -7072,46 +7092,46 @@
   </sheetPr>
   <dimension ref="A1:AL3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:AL3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="51.85546875" style="89" customWidth="1"/>
-    <col min="8" max="8" width="39.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="89" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28" style="89" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30.5703125" style="89" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="29.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="41.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="27" style="89" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="26.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="28.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="25.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="29.85546875" style="89" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="20.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="32.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.140625" style="89" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="30.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="25.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16" style="89" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.28515625" style="89" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="23.7109375" style="89" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="19.28515625" style="89" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="51.85546875" style="86" customWidth="1"/>
+    <col min="8" max="8" width="39.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="86" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28" style="86" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.5703125" style="86" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="41.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27" style="86" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="28.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="25.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="29.85546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="32.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.140625" style="86" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="30.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="25.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16" style="86" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.28515625" style="86" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.42578125" style="86" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="23.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="19.28515625" style="86" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" s="56" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7124,10 +7144,10 @@
       <c r="C1" s="45" t="s">
         <v>258</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="118" t="s">
         <v>260</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="118" t="s">
         <v>261</v>
       </c>
       <c r="F1" s="76" t="s">
@@ -7211,217 +7231,226 @@
       <c r="AF1" s="56" t="s">
         <v>622</v>
       </c>
-      <c r="AG1" s="87" t="s">
+      <c r="AG1" s="119" t="s">
         <v>514</v>
       </c>
-      <c r="AH1" s="87" t="s">
+      <c r="AH1" s="119" t="s">
         <v>515</v>
       </c>
-      <c r="AI1" s="87" t="s">
+      <c r="AI1" s="119" t="s">
         <v>516</v>
       </c>
-      <c r="AJ1" s="87" t="s">
+      <c r="AJ1" s="119" t="s">
         <v>517</v>
       </c>
-      <c r="AK1" s="87" t="s">
+      <c r="AK1" s="119" t="s">
         <v>518</v>
       </c>
-      <c r="AL1" s="87" t="s">
+      <c r="AL1" s="119" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="2" spans="1:38" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="120" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="121" t="s">
         <v>640</v>
       </c>
-      <c r="C2" s="88" t="s">
+      <c r="C2" s="116" t="s">
         <v>348</v>
       </c>
-      <c r="D2" s="88" t="s">
+      <c r="D2" s="116" t="s">
         <v>350</v>
       </c>
-      <c r="E2" s="88" t="s">
+      <c r="E2" s="116" t="s">
         <v>351</v>
       </c>
-      <c r="F2" s="88" t="s">
+      <c r="F2" s="116" t="s">
         <v>146</v>
       </c>
-      <c r="G2" s="82" t="s">
+      <c r="G2" s="120" t="s">
         <v>641</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="117" t="s">
         <v>460</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="117" t="s">
         <v>361</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="117" t="s">
         <v>134</v>
       </c>
-      <c r="K2" s="103" t="s">
+      <c r="K2" s="122" t="s">
         <v>455</v>
       </c>
-      <c r="L2" s="103" t="s">
+      <c r="L2" s="122" t="s">
         <v>642</v>
       </c>
-      <c r="M2" s="103" t="s">
+      <c r="M2" s="122" t="s">
         <v>457</v>
       </c>
-      <c r="N2" s="104" t="s">
+      <c r="N2" s="123" t="s">
         <v>643</v>
       </c>
-      <c r="O2" s="104"/>
-      <c r="P2" s="104" t="s">
+      <c r="O2" s="123"/>
+      <c r="P2" s="123" t="s">
         <v>644</v>
       </c>
-      <c r="Q2" s="103" t="s">
+      <c r="Q2" s="122" t="s">
         <v>645</v>
       </c>
-      <c r="R2" s="104"/>
-      <c r="S2" s="104"/>
-      <c r="T2" s="104" t="s">
+      <c r="R2" s="123"/>
+      <c r="S2" s="123"/>
+      <c r="T2" s="123" t="s">
         <v>646</v>
       </c>
-      <c r="U2" s="103" t="s">
+      <c r="U2" s="122" t="s">
         <v>455</v>
       </c>
-      <c r="V2" s="103" t="s">
+      <c r="V2" s="122" t="s">
         <v>455</v>
       </c>
-      <c r="W2" s="103" t="s">
+      <c r="W2" s="122" t="s">
         <v>455</v>
       </c>
-      <c r="X2" s="103" t="s">
+      <c r="X2" s="122" t="s">
         <v>455</v>
       </c>
-      <c r="Y2" s="103" t="s">
+      <c r="Y2" s="122" t="s">
         <v>647</v>
       </c>
-      <c r="Z2" s="84" t="s">
+      <c r="Z2" s="124" t="s">
         <v>648</v>
       </c>
-      <c r="AA2" s="103" t="s">
+      <c r="AA2" s="122" t="s">
         <v>649</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AB2" s="117" t="s">
         <v>650</v>
       </c>
-      <c r="AC2" s="104" t="s">
+      <c r="AC2" s="123" t="s">
         <v>651</v>
       </c>
-      <c r="AD2" s="103" t="s">
+      <c r="AD2" s="122" t="s">
         <v>647</v>
       </c>
-      <c r="AE2" s="105"/>
-      <c r="AF2" s="48" t="s">
+      <c r="AE2" s="125"/>
+      <c r="AF2" s="126" t="s">
         <v>643</v>
       </c>
+      <c r="AG2" s="127"/>
+      <c r="AH2" s="127"/>
+      <c r="AI2" s="127"/>
+      <c r="AJ2" s="127"/>
+      <c r="AK2" s="127"/>
+      <c r="AL2" s="127"/>
     </row>
     <row r="3" spans="1:38" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="120" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="121" t="s">
         <v>652</v>
       </c>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="116" t="s">
         <v>348</v>
       </c>
-      <c r="D3" s="88" t="s">
+      <c r="D3" s="116" t="s">
         <v>350</v>
       </c>
-      <c r="E3" s="88" t="s">
+      <c r="E3" s="116" t="s">
         <v>351</v>
       </c>
-      <c r="F3" s="88" t="s">
+      <c r="F3" s="116" t="s">
         <v>116</v>
       </c>
-      <c r="G3" s="82">
+      <c r="G3" s="120">
         <v>60003007</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="117" t="s">
         <v>460</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="117" t="s">
         <v>361</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="117" t="s">
         <v>134</v>
       </c>
-      <c r="K3" s="84" t="s">
+      <c r="K3" s="124" t="s">
         <v>653</v>
       </c>
-      <c r="L3" s="84" t="s">
+      <c r="L3" s="124" t="s">
         <v>522</v>
       </c>
-      <c r="M3" s="84" t="s">
+      <c r="M3" s="124" t="s">
         <v>459</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="117" t="s">
         <v>654</v>
       </c>
-      <c r="P3" t="s">
+      <c r="O3" s="127"/>
+      <c r="P3" s="117" t="s">
         <v>644</v>
       </c>
-      <c r="Q3" s="84" t="s">
+      <c r="Q3" s="124" t="s">
         <v>655</v>
       </c>
-      <c r="T3" t="s">
+      <c r="R3" s="127"/>
+      <c r="S3" s="127"/>
+      <c r="T3" s="117" t="s">
         <v>646</v>
       </c>
-      <c r="U3" s="84" t="s">
+      <c r="U3" s="124" t="s">
         <v>653</v>
       </c>
-      <c r="V3" s="84" t="s">
+      <c r="V3" s="124" t="s">
         <v>653</v>
       </c>
-      <c r="W3" s="84" t="s">
+      <c r="W3" s="124" t="s">
         <v>653</v>
       </c>
-      <c r="X3" s="84" t="s">
+      <c r="X3" s="124" t="s">
         <v>653</v>
       </c>
-      <c r="Y3" s="84" t="s">
+      <c r="Y3" s="124" t="s">
         <v>656</v>
       </c>
-      <c r="Z3" s="84" t="s">
+      <c r="Z3" s="124" t="s">
         <v>648</v>
       </c>
-      <c r="AA3" s="84" t="s">
+      <c r="AA3" s="124" t="s">
         <v>656</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AB3" s="117" t="s">
         <v>650</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AC3" s="117" t="s">
         <v>654</v>
       </c>
-      <c r="AD3" s="84" t="s">
+      <c r="AD3" s="124" t="s">
         <v>656</v>
       </c>
-      <c r="AE3" s="85"/>
-      <c r="AF3" s="88" t="s">
+      <c r="AE3" s="128"/>
+      <c r="AF3" s="116" t="s">
         <v>654</v>
       </c>
-      <c r="AG3" s="90" t="s">
+      <c r="AG3" s="87" t="s">
         <v>94</v>
       </c>
-      <c r="AH3" s="84" t="s">
+      <c r="AH3" s="124" t="s">
         <v>522</v>
       </c>
-      <c r="AI3" s="84" t="s">
+      <c r="AI3" s="124" t="s">
         <v>525</v>
       </c>
-      <c r="AJ3" s="84" t="s">
+      <c r="AJ3" s="124" t="s">
         <v>522</v>
       </c>
-      <c r="AK3" s="84" t="s">
+      <c r="AK3" s="124" t="s">
         <v>657</v>
       </c>
-      <c r="AL3" s="84" t="s">
+      <c r="AL3" s="124" t="s">
         <v>543</v>
       </c>
     </row>

</xml_diff>